<commit_message>
Updated to Version 1.1 for software
* Fixed an error in the set current function of the DAC
* Added improved current calculation to allow for correction in OP-AMP
offset, uses the measured value to adjust the set current.
* General code tidy up

Added a few things to the BOM that I had forgotten
</commit_message>
<xml_diff>
--- a/Design Spark/rev 2/Dummy Load Rev 2 (Bill Of Materials).xlsx
+++ b/Design Spark/rev 2/Dummy Load Rev 2 (Bill Of Materials).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="224">
   <si>
     <t>Ref Name</t>
   </si>
@@ -681,6 +681,12 @@
   </si>
   <si>
     <t>Cannot Find</t>
+  </si>
+  <si>
+    <t>Binding Post - Black</t>
+  </si>
+  <si>
+    <t>Binding Post - Red</t>
   </si>
 </sst>
 </file>
@@ -1189,13 +1195,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1538,10 +1544,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2962,7 +2968,7 @@
       <c r="G56" t="s">
         <v>102</v>
       </c>
-      <c r="J56" s="7">
+      <c r="J56" s="6">
         <v>111428926233</v>
       </c>
     </row>
@@ -2985,7 +2991,7 @@
       <c r="G57" t="s">
         <v>102</v>
       </c>
-      <c r="J57" s="7">
+      <c r="J57" s="6">
         <v>111428926233</v>
       </c>
     </row>
@@ -3008,7 +3014,7 @@
       <c r="G58" t="s">
         <v>102</v>
       </c>
-      <c r="J58" s="7">
+      <c r="J58" s="6">
         <v>111428926233</v>
       </c>
     </row>
@@ -3089,7 +3095,7 @@
       <c r="G61" t="s">
         <v>102</v>
       </c>
-      <c r="J61" s="6" t="s">
+      <c r="J61" s="8" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3112,7 +3118,7 @@
       <c r="G62" t="s">
         <v>102</v>
       </c>
-      <c r="J62" s="6"/>
+      <c r="J62" s="8"/>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
@@ -3133,7 +3139,7 @@
       <c r="G63" t="s">
         <v>102</v>
       </c>
-      <c r="J63" s="6"/>
+      <c r="J63" s="8"/>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
@@ -3154,7 +3160,7 @@
       <c r="G64" t="s">
         <v>102</v>
       </c>
-      <c r="J64" s="6"/>
+      <c r="J64" s="8"/>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
@@ -3175,7 +3181,7 @@
       <c r="G65" t="s">
         <v>102</v>
       </c>
-      <c r="J65" s="6"/>
+      <c r="J65" s="8"/>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
@@ -3196,7 +3202,7 @@
       <c r="G66" t="s">
         <v>102</v>
       </c>
-      <c r="J66" s="6"/>
+      <c r="J66" s="8"/>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
@@ -3217,7 +3223,7 @@
       <c r="G67" t="s">
         <v>102</v>
       </c>
-      <c r="J67" s="6"/>
+      <c r="J67" s="8"/>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
@@ -3238,7 +3244,7 @@
       <c r="G68" t="s">
         <v>102</v>
       </c>
-      <c r="J68" s="6"/>
+      <c r="J68" s="8"/>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
@@ -3259,7 +3265,7 @@
       <c r="G69" t="s">
         <v>102</v>
       </c>
-      <c r="J69" s="6"/>
+      <c r="J69" s="8"/>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
@@ -3280,7 +3286,7 @@
       <c r="G70" t="s">
         <v>102</v>
       </c>
-      <c r="J70" s="6"/>
+      <c r="J70" s="8"/>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
@@ -3301,7 +3307,7 @@
       <c r="G71" t="s">
         <v>102</v>
       </c>
-      <c r="J71" s="6"/>
+      <c r="J71" s="8"/>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
@@ -3322,7 +3328,7 @@
       <c r="G72" t="s">
         <v>102</v>
       </c>
-      <c r="J72" s="7">
+      <c r="J72" s="6">
         <v>111428926233</v>
       </c>
     </row>
@@ -3371,7 +3377,7 @@
       <c r="G74" t="s">
         <v>102</v>
       </c>
-      <c r="J74" s="7">
+      <c r="J74" s="6">
         <v>111428926233</v>
       </c>
     </row>
@@ -3837,7 +3843,7 @@
       <c r="C100" t="s">
         <v>213</v>
       </c>
-      <c r="E100" s="8" t="s">
+      <c r="E100" s="7" t="s">
         <v>214</v>
       </c>
       <c r="H100" s="4">
@@ -3854,7 +3860,7 @@
       <c r="C101" t="s">
         <v>215</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="E101" s="7" t="s">
         <v>216</v>
       </c>
       <c r="H101" s="4">
@@ -3869,7 +3875,7 @@
       <c r="C102" t="s">
         <v>217</v>
       </c>
-      <c r="E102" s="8" t="s">
+      <c r="E102" s="7" t="s">
         <v>218</v>
       </c>
       <c r="H102" s="4">
@@ -3884,13 +3890,35 @@
       <c r="C103" t="s">
         <v>219</v>
       </c>
-      <c r="E103" s="8" t="s">
+      <c r="E103" s="7" t="s">
         <v>220</v>
       </c>
       <c r="H103" s="4">
         <v>1782871</v>
       </c>
       <c r="I103" s="9"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>222</v>
+      </c>
+      <c r="H104" s="4">
+        <v>173711301</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105" t="s">
+        <v>223</v>
+      </c>
+      <c r="H105" s="4">
+        <v>173711201</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A13:I110">
@@ -4033,8 +4061,10 @@
     <hyperlink ref="J57" r:id="rId130" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
     <hyperlink ref="J56" r:id="rId131" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
     <hyperlink ref="J74" r:id="rId132" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
+    <hyperlink ref="H104" r:id="rId133" display="http://au.element14.com/jsp/search/productdetail.jsp?id=1737113&amp;Ntt=173711301&amp;whydiditmatch=clone&amp;matchedProduct=173711301"/>
+    <hyperlink ref="H105" r:id="rId134" display="http://au.element14.com/cliff-electronic-components/tp-6s-red-assembled/binding-post-30a-4mm-panel-red/dp/1737112?Ntt=173711201&amp;whydiditmatch=clone&amp;matchedProduct=173711201"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId133"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId135"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Top Solder Paste Stencil
Added paste stencil and minor chances to BOM
</commit_message>
<xml_diff>
--- a/Design Spark/rev 2/Dummy Load Rev 2 (Bill Of Materials).xlsx
+++ b/Design Spark/rev 2/Dummy Load Rev 2 (Bill Of Materials).xlsx
@@ -1546,8 +1546,8 @@
   </sheetPr>
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J77" sqref="J77:J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2549,7 +2549,7 @@
         <v>60</v>
       </c>
       <c r="J41" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2569,7 +2569,7 @@
         <v>60</v>
       </c>
       <c r="J42" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -3432,7 +3432,7 @@
         <v>64</v>
       </c>
       <c r="J77" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -3449,7 +3449,7 @@
         <v>64</v>
       </c>
       <c r="J78" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -3466,7 +3466,7 @@
         <v>64</v>
       </c>
       <c r="J79" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -3483,7 +3483,7 @@
         <v>64</v>
       </c>
       <c r="J80" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3500,7 +3500,7 @@
         <v>64</v>
       </c>
       <c r="J81" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3517,7 +3517,7 @@
         <v>64</v>
       </c>
       <c r="J82" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3534,7 +3534,7 @@
         <v>64</v>
       </c>
       <c r="J83" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3551,7 +3551,7 @@
         <v>64</v>
       </c>
       <c r="J84" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3568,7 +3568,7 @@
         <v>64</v>
       </c>
       <c r="J85" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3585,7 +3585,7 @@
         <v>64</v>
       </c>
       <c r="J86" s="5">
-        <v>371104220164</v>
+        <v>251273258816</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -4042,27 +4042,27 @@
     <hyperlink ref="I97" r:id="rId111" display="http://www.digikey.com/product-detail/en/CG0603MLC-05E/CG0603MLC-05ECT-ND/3438061"/>
     <hyperlink ref="J31" r:id="rId112" display="http://www.ebay.com/sch/i.html?_from=R40&amp;_trksid=p2050601.m570.l1313.TR11.TRC1.A0.H0.Xrotary+encoder&amp;_nkw=rotary+encoder&amp;_sacat=0"/>
     <hyperlink ref="J36" r:id="rId113" display="http://www.ebay.com/itm/2004-204-20x4-Character-LCD-Display-Module-HD44780-Controller-Blue-Blacklight-/400448319287?pt=LH_DefaultDomain_0&amp;hash=item5d3c946f37"/>
-    <hyperlink ref="J41" r:id="rId114" display="http://www.ebay.com/itm/10x-Male-40-Pin-Single-Row-0-1-2-54mm-Pitch-Breakable-Header-/371104220164?pt=LH_DefaultDomain_0&amp;hash=item5667890404"/>
-    <hyperlink ref="J42" r:id="rId115" display="http://www.ebay.com/itm/10x-Male-40-Pin-Single-Row-0-1-2-54mm-Pitch-Breakable-Header-/371104220164?pt=LH_DefaultDomain_0&amp;hash=item5667890404"/>
-    <hyperlink ref="J72" r:id="rId116" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
-    <hyperlink ref="I73" r:id="rId117" display="http://au.element14.com/bourns/3362p-1-103lf/pot-trimmer-10k-3-pin/dp/9354301"/>
-    <hyperlink ref="J73" r:id="rId118" display="http://www.digikey.com/product-detail/en/3362P-1-103LF/3362P-103LF-ND/1088412"/>
-    <hyperlink ref="J77" r:id="rId119" display="http://www.ebay.com/itm/10x-Male-40-Pin-Single-Row-0-1-2-54mm-Pitch-Breakable-Header-/371104220164?pt=LH_DefaultDomain_0&amp;hash=item5667890404"/>
-    <hyperlink ref="J78:J86" r:id="rId120" display="http://www.ebay.com/itm/10x-Male-40-Pin-Single-Row-0-1-2-54mm-Pitch-Breakable-Header-/371104220164?pt=LH_DefaultDomain_0&amp;hash=item5667890404"/>
-    <hyperlink ref="J76" r:id="rId121" display="http://www.ebay.com/itm/100pcs-Tactile-Pushbutton-Switch-Momentary-Tact-LCD-Screen-Monitor-4pin-6-6-5mm-/221432348499?pt=LH_DefaultDomain_0&amp;hash=item338e657f53"/>
-    <hyperlink ref="H98" r:id="rId122" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1466932"/>
-    <hyperlink ref="I98" r:id="rId123" display="http://www.digikey.com/product-detail/en/9072/9072-ND/4499377"/>
-    <hyperlink ref="J99" r:id="rId124" display="http://www.ebay.com/itm/50-pcs-M3-x-6mm-Philips-Head-Screw-/350820635884?pt=LH_DefaultDomain_0&amp;hash=item51ae8a14ec"/>
-    <hyperlink ref="H100" r:id="rId125" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1773364"/>
-    <hyperlink ref="H101" r:id="rId126" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1773348"/>
-    <hyperlink ref="H102" r:id="rId127" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1219149"/>
-    <hyperlink ref="H103" r:id="rId128" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1782871"/>
-    <hyperlink ref="J58" r:id="rId129" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
-    <hyperlink ref="J57" r:id="rId130" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
-    <hyperlink ref="J56" r:id="rId131" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
-    <hyperlink ref="J74" r:id="rId132" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
-    <hyperlink ref="H104" r:id="rId133" display="http://au.element14.com/jsp/search/productdetail.jsp?id=1737113&amp;Ntt=173711301&amp;whydiditmatch=clone&amp;matchedProduct=173711301"/>
-    <hyperlink ref="H105" r:id="rId134" display="http://au.element14.com/cliff-electronic-components/tp-6s-red-assembled/binding-post-30a-4mm-panel-red/dp/1737112?Ntt=173711201&amp;whydiditmatch=clone&amp;matchedProduct=173711201"/>
+    <hyperlink ref="J72" r:id="rId114" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
+    <hyperlink ref="I73" r:id="rId115" display="http://au.element14.com/bourns/3362p-1-103lf/pot-trimmer-10k-3-pin/dp/9354301"/>
+    <hyperlink ref="J73" r:id="rId116" display="http://www.digikey.com/product-detail/en/3362P-1-103LF/3362P-103LF-ND/1088412"/>
+    <hyperlink ref="J76" r:id="rId117" display="http://www.ebay.com/itm/100pcs-Tactile-Pushbutton-Switch-Momentary-Tact-LCD-Screen-Monitor-4pin-6-6-5mm-/221432348499?pt=LH_DefaultDomain_0&amp;hash=item338e657f53"/>
+    <hyperlink ref="H98" r:id="rId118" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1466932"/>
+    <hyperlink ref="I98" r:id="rId119" display="http://www.digikey.com/product-detail/en/9072/9072-ND/4499377"/>
+    <hyperlink ref="J99" r:id="rId120" display="http://www.ebay.com/itm/50-pcs-M3-x-6mm-Philips-Head-Screw-/350820635884?pt=LH_DefaultDomain_0&amp;hash=item51ae8a14ec"/>
+    <hyperlink ref="H100" r:id="rId121" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1773364"/>
+    <hyperlink ref="H101" r:id="rId122" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1773348"/>
+    <hyperlink ref="H102" r:id="rId123" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1219149"/>
+    <hyperlink ref="H103" r:id="rId124" display="https://au.element14.com/jsp/search/productdetail.jsp?SKU=1782871"/>
+    <hyperlink ref="J58" r:id="rId125" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
+    <hyperlink ref="J57" r:id="rId126" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
+    <hyperlink ref="J56" r:id="rId127" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
+    <hyperlink ref="J74" r:id="rId128" display="http://www.ebay.com/itm/0805-E12-SMDR-SMD-Resistor-Assorted-Kit-86-values-x-50-5-4300pcs-New-/111428926233?pt=LH_DefaultDomain_0&amp;hash=item19f1ae7b19"/>
+    <hyperlink ref="H104" r:id="rId129" display="http://au.element14.com/jsp/search/productdetail.jsp?id=1737113&amp;Ntt=173711301&amp;whydiditmatch=clone&amp;matchedProduct=173711301"/>
+    <hyperlink ref="H105" r:id="rId130" display="http://au.element14.com/cliff-electronic-components/tp-6s-red-assembled/binding-post-30a-4mm-panel-red/dp/1737112?Ntt=173711201&amp;whydiditmatch=clone&amp;matchedProduct=173711201"/>
+    <hyperlink ref="J41" r:id="rId131" display="http://www.ebay.com.au/itm/New-40-Pin-2-54mm-Male-Female-SIL-Header-Socket-Single-Row-Strip-PCB-Connector-/251273258816?pt=AU_B_I_Electrical_Test_Equipment&amp;hash=item3a810da740&amp;_uhb=1"/>
+    <hyperlink ref="J42" r:id="rId132" display="http://www.ebay.com.au/itm/New-40-Pin-2-54mm-Male-Female-SIL-Header-Socket-Single-Row-Strip-PCB-Connector-/251273258816?pt=AU_B_I_Electrical_Test_Equipment&amp;hash=item3a810da740&amp;_uhb=1"/>
+    <hyperlink ref="J77" r:id="rId133" display="http://www.ebay.com.au/itm/New-40-Pin-2-54mm-Male-Female-SIL-Header-Socket-Single-Row-Strip-PCB-Connector-/251273258816?pt=AU_B_I_Electrical_Test_Equipment&amp;hash=item3a810da740&amp;_uhb=1"/>
+    <hyperlink ref="J78:J86" r:id="rId134" display="http://www.ebay.com.au/itm/New-40-Pin-2-54mm-Male-Female-SIL-Header-Socket-Single-Row-Strip-PCB-Connector-/251273258816?pt=AU_B_I_Electrical_Test_Equipment&amp;hash=item3a810da740&amp;_uhb=1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId135"/>

</xml_diff>